<commit_message>
Bug fixes to RED code
</commit_message>
<xml_diff>
--- a/working/SmeltzPFAS/SmeltzPFAS-fup-RED-Level4.xlsx
+++ b/working/SmeltzPFAS/SmeltzPFAS-fup-RED-Level4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwambaug\git\invitrotkstats\working\SmeltzPFAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{589B9E61-A26B-4778-926F-9DE7FFABBF5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3797A8CA-8B3A-4E01-80B8-5E76D46EFAC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37245" yWindow="2010" windowWidth="19425" windowHeight="11025"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440"/>
   </bookViews>
   <sheets>
     <sheet name="SmeltzPFAS-fup-RED-Level4" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="51">
   <si>
     <t>Compound.Name</t>
   </si>
@@ -127,12 +127,6 @@
     <t>DTXSID1037303</t>
   </si>
   <si>
-    <t>8:2 Fluorotelomer sulfonic acid</t>
-  </si>
-  <si>
-    <t>DTXSID00192353</t>
-  </si>
-  <si>
     <t>Perfluoroundecanoic acid</t>
   </si>
   <si>
@@ -173,6 +167,12 @@
   </si>
   <si>
     <t>DTXSID50375114</t>
+  </si>
+  <si>
+    <t>Uncertain</t>
+  </si>
+  <si>
+    <t>CV</t>
   </si>
 </sst>
 </file>
@@ -315,7 +315,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -495,8 +495,14 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -611,6 +617,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -656,9 +671,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -704,12 +721,37 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
     <dxf>
-      <numFmt numFmtId="15" formatCode="0.00E+00"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="15" formatCode="0.00E+00"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <right style="thin">
+          <color theme="4"/>
+        </right>
+      </border>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -725,16 +767,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G23" totalsRowShown="0">
-  <autoFilter ref="A1:G23"/>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:I22" totalsRowShown="0" tableBorderDxfId="2">
+  <autoFilter ref="A1:I22"/>
+  <tableColumns count="9">
     <tableColumn id="1" name="Compound.Name"/>
     <tableColumn id="2" name="Lab.Compound.Name"/>
     <tableColumn id="3" name="DTXSID"/>
     <tableColumn id="4" name="Fup.point"/>
-    <tableColumn id="5" name="Fup.Med" dataDxfId="1"/>
-    <tableColumn id="6" name="Fup.Low" dataDxfId="0"/>
+    <tableColumn id="5" name="Fup.Med"/>
+    <tableColumn id="6" name="Fup.Low"/>
     <tableColumn id="7" name="Fup.High"/>
+    <tableColumn id="8" name="Uncertain" dataDxfId="1">
+      <calculatedColumnFormula>IF((LOG10(G2)-LOG10(F2))&gt;3,"Y","")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" name="CV" dataDxfId="0">
+      <calculatedColumnFormula>(G2-F2)/1.96/E2</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1037,10 +1085,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G23"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1052,9 +1100,10 @@
     <col min="5" max="5" width="10.36328125" customWidth="1"/>
     <col min="6" max="6" width="10" customWidth="1"/>
     <col min="7" max="7" width="10.36328125" customWidth="1"/>
+    <col min="8" max="8" width="11.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1076,8 +1125,14 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1088,19 +1143,27 @@
         <v>8</v>
       </c>
       <c r="D2">
-        <v>1.636E-2</v>
+        <v>2.7740000000000001E-2</v>
       </c>
       <c r="E2">
-        <v>1.5480000000000001E-2</v>
+        <v>1.444E-2</v>
       </c>
       <c r="F2">
-        <v>1.227E-2</v>
+        <v>1.0959999999999999E-2</v>
       </c>
       <c r="G2">
-        <v>2.0410000000000001E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+        <v>1.9060000000000001E-2</v>
+      </c>
+      <c r="H2" s="3" t="str">
+        <f>IF((LOG10(G2)-LOG10(F2))&gt;3,"Y","")</f>
+        <v/>
+      </c>
+      <c r="I2" s="3">
+        <f>(G2-F2)/1.96/E2</f>
+        <v>0.28619481033410604</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1111,19 +1174,27 @@
         <v>10</v>
       </c>
       <c r="D3">
-        <v>4.5409999999999999E-2</v>
+        <v>5.1209999999999999E-2</v>
       </c>
       <c r="E3">
-        <v>4.4810000000000003E-2</v>
+        <v>4.2979999999999997E-2</v>
       </c>
       <c r="F3">
-        <v>3.2480000000000002E-2</v>
+        <v>2.9059999999999999E-2</v>
       </c>
       <c r="G3">
-        <v>6.6000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+        <v>6.3710000000000003E-2</v>
+      </c>
+      <c r="H3" s="3" t="str">
+        <f t="shared" ref="H3:H22" si="0">IF((LOG10(G3)-LOG10(F3))&gt;3,"Y","")</f>
+        <v/>
+      </c>
+      <c r="I3" s="3">
+        <f t="shared" ref="I3:I22" si="1">(G3-F3)/1.96/E3</f>
+        <v>0.41132088014358842</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1134,19 +1205,27 @@
         <v>12</v>
       </c>
       <c r="D4">
-        <v>1.1270000000000001E-2</v>
+        <v>1.3429999999999999E-2</v>
       </c>
       <c r="E4">
-        <v>1.1780000000000001E-2</v>
+        <v>1.112E-2</v>
       </c>
       <c r="F4">
-        <v>8.3149999999999995E-3</v>
+        <v>7.7010000000000004E-3</v>
       </c>
       <c r="G4">
-        <v>1.755E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+        <v>1.6400000000000001E-2</v>
+      </c>
+      <c r="H4" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I4" s="3">
+        <f t="shared" si="1"/>
+        <v>0.39912457788870953</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -1157,19 +1236,27 @@
         <v>14</v>
       </c>
       <c r="D5">
-        <v>4.2599999999999999E-3</v>
-      </c>
-      <c r="E5" s="1">
-        <v>4.1419999999999999E-7</v>
-      </c>
-      <c r="F5" s="1">
-        <v>1.4179999999999999E-10</v>
+        <v>8.1609999999999999E-3</v>
+      </c>
+      <c r="E5">
+        <v>2.2390000000000001E-3</v>
+      </c>
+      <c r="F5">
+        <v>1.6019999999999999E-3</v>
       </c>
       <c r="G5">
-        <v>2.1689999999999999E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+        <v>3.0799999999999998E-3</v>
+      </c>
+      <c r="H5" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I5" s="3">
+        <f t="shared" si="1"/>
+        <v>0.33679394044352889</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -1180,19 +1267,27 @@
         <v>16</v>
       </c>
       <c r="D6">
-        <v>1.008E-3</v>
-      </c>
-      <c r="E6" s="1">
-        <v>4.3000000000000001E-7</v>
-      </c>
-      <c r="F6" s="1">
-        <v>1.458E-10</v>
+        <v>1.0300000000000001E-3</v>
+      </c>
+      <c r="E6">
+        <v>1.5319999999999999E-3</v>
+      </c>
+      <c r="F6">
+        <v>9.5870000000000005E-4</v>
       </c>
       <c r="G6">
-        <v>8.9749999999999997E-4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+        <v>4.712E-3</v>
+      </c>
+      <c r="H6" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I6" s="3">
+        <f t="shared" si="1"/>
+        <v>1.2499666968615124</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -1203,19 +1298,27 @@
         <v>18</v>
       </c>
       <c r="D7">
-        <v>4.5449999999999999E-4</v>
-      </c>
-      <c r="E7" s="1">
-        <v>4.3230000000000003E-7</v>
-      </c>
-      <c r="F7" s="1">
-        <v>1.4430000000000001E-10</v>
+        <v>7.6000000000000004E-4</v>
+      </c>
+      <c r="E7">
+        <v>2.5549999999999998E-4</v>
+      </c>
+      <c r="F7">
+        <v>1.727E-4</v>
       </c>
       <c r="G7">
-        <v>3.3599999999999998E-4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+        <v>3.725E-4</v>
+      </c>
+      <c r="H7" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I7" s="3">
+        <f t="shared" si="1"/>
+        <v>0.39897759495187513</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -1226,19 +1329,27 @@
         <v>20</v>
       </c>
       <c r="D8">
-        <v>2.0109999999999999E-2</v>
+        <v>2.5049999999999999E-2</v>
       </c>
       <c r="E8">
-        <v>1.9550000000000001E-2</v>
+        <v>1.9140000000000001E-2</v>
       </c>
       <c r="F8">
-        <v>1.585E-2</v>
+        <v>1.5599999999999999E-2</v>
       </c>
       <c r="G8">
-        <v>2.3789999999999999E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+        <v>2.3189999999999999E-2</v>
+      </c>
+      <c r="H8" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I8" s="3">
+        <f t="shared" si="1"/>
+        <v>0.20232230823363825</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -1248,20 +1359,28 @@
       <c r="C9" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="1">
-        <v>7.6710000000000002E-5</v>
+      <c r="D9">
+        <v>1.2530000000000001E-4</v>
       </c>
       <c r="E9" s="1">
-        <v>2.1409999999999999E-7</v>
+        <v>7.7529999999999998E-5</v>
       </c>
       <c r="F9" s="1">
-        <v>1.5350000000000001E-10</v>
-      </c>
-      <c r="G9" s="1">
-        <v>9.3140000000000006E-5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+        <v>4.9960000000000003E-5</v>
+      </c>
+      <c r="G9">
+        <v>1.175E-4</v>
+      </c>
+      <c r="H9" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I9" s="3">
+        <f t="shared" si="1"/>
+        <v>0.44446257801456712</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -1272,19 +1391,27 @@
         <v>24</v>
       </c>
       <c r="D10">
-        <v>0.124</v>
+        <v>0.12470000000000001</v>
       </c>
       <c r="E10">
-        <v>0.13100000000000001</v>
+        <v>0.1313</v>
       </c>
       <c r="F10">
-        <v>8.8029999999999997E-2</v>
+        <v>8.6300000000000002E-2</v>
       </c>
       <c r="G10">
-        <v>0.19370000000000001</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+        <v>0.19170000000000001</v>
+      </c>
+      <c r="H10" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I10" s="3">
+        <f t="shared" si="1"/>
+        <v>0.40956214930755247</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -1295,19 +1422,27 @@
         <v>26</v>
       </c>
       <c r="D11">
-        <v>2.9859999999999999E-4</v>
-      </c>
-      <c r="E11" s="1">
-        <v>7.5059999999999996E-7</v>
-      </c>
-      <c r="F11" s="1">
-        <v>1.5729999999999999E-10</v>
+        <v>4.528E-4</v>
+      </c>
+      <c r="E11">
+        <v>2.186E-4</v>
+      </c>
+      <c r="F11">
+        <v>1.507E-4</v>
       </c>
       <c r="G11">
-        <v>3.0600000000000001E-4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+        <v>3.1789999999999998E-4</v>
+      </c>
+      <c r="H11" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I11" s="3">
+        <f t="shared" si="1"/>
+        <v>0.39023843755251408</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -1318,19 +1453,27 @@
         <v>28</v>
       </c>
       <c r="D12">
-        <v>9.0379999999999996E-4</v>
-      </c>
-      <c r="E12" s="1">
-        <v>3.3710000000000002E-7</v>
-      </c>
-      <c r="F12" s="1">
-        <v>1.6740000000000001E-10</v>
+        <v>9.5450000000000005E-4</v>
+      </c>
+      <c r="E12">
+        <v>7.963E-4</v>
+      </c>
+      <c r="F12">
+        <v>5.5099999999999995E-4</v>
       </c>
       <c r="G12">
-        <v>6.9970000000000004E-4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+        <v>1.1820000000000001E-3</v>
+      </c>
+      <c r="H12" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I12" s="3">
+        <f t="shared" si="1"/>
+        <v>0.40429332602060047</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -1341,19 +1484,27 @@
         <v>30</v>
       </c>
       <c r="D13">
-        <v>1.591E-3</v>
-      </c>
-      <c r="E13" s="1">
-        <v>2.7420000000000001E-7</v>
-      </c>
-      <c r="F13" s="1">
-        <v>1.4960000000000001E-10</v>
+        <v>2.6329999999999999E-3</v>
+      </c>
+      <c r="E13">
+        <v>7.961E-4</v>
+      </c>
+      <c r="F13">
+        <v>5.4319999999999998E-4</v>
       </c>
       <c r="G13">
-        <v>8.6370000000000001E-4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+        <v>1.152E-3</v>
+      </c>
+      <c r="H13" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I13" s="3">
+        <f t="shared" si="1"/>
+        <v>0.39016737206124757</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -1364,19 +1515,27 @@
         <v>32</v>
       </c>
       <c r="D14">
-        <v>1.034E-2</v>
+        <v>1.401E-2</v>
       </c>
       <c r="E14">
-        <v>1.0999999999999999E-2</v>
+        <v>1.074E-2</v>
       </c>
       <c r="F14">
-        <v>7.5570000000000003E-3</v>
+        <v>7.3340000000000002E-3</v>
       </c>
       <c r="G14">
-        <v>1.6379999999999999E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+        <v>1.5180000000000001E-2</v>
+      </c>
+      <c r="H14" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I14" s="3">
+        <f t="shared" si="1"/>
+        <v>0.37272450879793262</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -1387,19 +1546,27 @@
         <v>34</v>
       </c>
       <c r="D15">
-        <v>1.1460000000000001E-3</v>
-      </c>
-      <c r="E15" s="1">
-        <v>5.0989999999999998E-7</v>
-      </c>
-      <c r="F15" s="1">
-        <v>1.5290000000000001E-10</v>
+        <v>2.4680000000000001E-3</v>
+      </c>
+      <c r="E15">
+        <v>1.7309999999999999E-3</v>
+      </c>
+      <c r="F15">
+        <v>1.1850000000000001E-3</v>
       </c>
       <c r="G15">
-        <v>1.524E-3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+        <v>2.47E-3</v>
+      </c>
+      <c r="H15" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I15" s="3">
+        <f t="shared" si="1"/>
+        <v>0.37874768624954319</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>35</v>
       </c>
@@ -1410,19 +1577,27 @@
         <v>36</v>
       </c>
       <c r="D16">
-        <v>9.2529999999999999E-4</v>
+        <v>4.3560000000000002E-4</v>
       </c>
       <c r="E16">
-        <v>1.6590000000000001E-3</v>
-      </c>
-      <c r="F16" s="1">
-        <v>5.0870000000000001E-10</v>
+        <v>1.9809999999999999E-4</v>
+      </c>
+      <c r="F16">
+        <v>1.3009999999999999E-4</v>
       </c>
       <c r="G16">
-        <v>5.7679999999999997E-3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+        <v>5.664E-4</v>
+      </c>
+      <c r="H16" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I16" s="3">
+        <f t="shared" si="1"/>
+        <v>1.1236852136109368</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>37</v>
       </c>
@@ -1432,20 +1607,28 @@
       <c r="C17" t="s">
         <v>38</v>
       </c>
-      <c r="D17">
-        <v>1.638E-4</v>
+      <c r="D17" s="1">
+        <v>4.7589999999999997E-5</v>
       </c>
       <c r="E17" s="1">
-        <v>1.222E-7</v>
+        <v>2.27E-5</v>
       </c>
       <c r="F17" s="1">
-        <v>1.4370000000000001E-10</v>
-      </c>
-      <c r="G17">
-        <v>1.4579999999999999E-4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+        <v>1.075E-5</v>
+      </c>
+      <c r="G17" s="1">
+        <v>5.5850000000000002E-5</v>
+      </c>
+      <c r="H17" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I17" s="3">
+        <f t="shared" si="1"/>
+        <v>1.0136653780454914</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>39</v>
       </c>
@@ -1455,20 +1638,28 @@
       <c r="C18" t="s">
         <v>40</v>
       </c>
-      <c r="D18" s="1">
-        <v>3.9759999999999999E-5</v>
-      </c>
-      <c r="E18" s="1">
-        <v>1.2270000000000001E-6</v>
-      </c>
-      <c r="F18" s="1">
-        <v>1.5720000000000001E-10</v>
-      </c>
-      <c r="G18" s="1">
-        <v>6.4380000000000004E-5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D18">
+        <v>4.875E-3</v>
+      </c>
+      <c r="E18">
+        <v>2.0939999999999999E-3</v>
+      </c>
+      <c r="F18">
+        <v>1.364E-3</v>
+      </c>
+      <c r="G18">
+        <v>5.47E-3</v>
+      </c>
+      <c r="H18" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I18" s="3">
+        <f t="shared" si="1"/>
+        <v>1.000428824825059</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>41</v>
       </c>
@@ -1479,19 +1670,27 @@
         <v>42</v>
       </c>
       <c r="D19">
-        <v>2.7550000000000001E-3</v>
-      </c>
-      <c r="E19" s="1">
-        <v>4.1209999999999999E-7</v>
-      </c>
-      <c r="F19" s="1">
-        <v>1.4970000000000001E-10</v>
+        <v>1.5299999999999999E-3</v>
+      </c>
+      <c r="E19">
+        <v>7.4859999999999998E-4</v>
+      </c>
+      <c r="F19">
+        <v>5.0810000000000004E-4</v>
       </c>
       <c r="G19">
-        <v>9.4660000000000002E-4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+        <v>1.0809999999999999E-3</v>
+      </c>
+      <c r="H19" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I19" s="3">
+        <f t="shared" si="1"/>
+        <v>0.39045674374478612</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>43</v>
       </c>
@@ -1502,19 +1701,27 @@
         <v>44</v>
       </c>
       <c r="D20">
-        <v>-1.985E-4</v>
-      </c>
-      <c r="E20" s="1">
-        <v>3.1590000000000002E-7</v>
-      </c>
-      <c r="F20" s="1">
-        <v>1.5610000000000001E-10</v>
+        <v>1.217E-2</v>
+      </c>
+      <c r="E20">
+        <v>3.392E-3</v>
+      </c>
+      <c r="F20">
+        <v>2.4529999999999999E-3</v>
       </c>
       <c r="G20">
-        <v>6.7809999999999995E-4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+        <v>4.6649999999999999E-3</v>
+      </c>
+      <c r="H20" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I20" s="3">
+        <f t="shared" si="1"/>
+        <v>0.33271563342318061</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>45</v>
       </c>
@@ -1525,19 +1732,27 @@
         <v>46</v>
       </c>
       <c r="D21">
-        <v>1.3159999999999999E-3</v>
-      </c>
-      <c r="E21" s="1">
-        <v>6.2020000000000001E-7</v>
-      </c>
-      <c r="F21" s="1">
-        <v>1.4339999999999999E-10</v>
+        <v>6.5749999999999999E-4</v>
+      </c>
+      <c r="E21">
+        <v>3.0449999999999997E-4</v>
+      </c>
+      <c r="F21">
+        <v>2.051E-4</v>
       </c>
       <c r="G21">
-        <v>2.3549999999999999E-3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+        <v>4.4549999999999999E-4</v>
+      </c>
+      <c r="H21" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I21" s="3">
+        <f t="shared" si="1"/>
+        <v>0.40280151469454784</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>47</v>
       </c>
@@ -1548,39 +1763,24 @@
         <v>48</v>
       </c>
       <c r="D22">
-        <v>4.572E-4</v>
+        <v>1.4129999999999999E-4</v>
       </c>
       <c r="E22" s="1">
-        <v>1.252E-6</v>
+        <v>4.8240000000000003E-7</v>
       </c>
       <c r="F22" s="1">
-        <v>1.544E-10</v>
+        <v>2.0550000000000001E-13</v>
       </c>
       <c r="G22">
-        <v>4.373E-4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>49</v>
-      </c>
-      <c r="B23" t="s">
-        <v>49</v>
-      </c>
-      <c r="C23" t="s">
-        <v>50</v>
-      </c>
-      <c r="D23">
-        <v>1.3109999999999999E-4</v>
-      </c>
-      <c r="E23" s="1">
-        <v>6.9690000000000005E-5</v>
-      </c>
-      <c r="F23" s="1">
-        <v>2.6559999999999999E-10</v>
-      </c>
-      <c r="G23">
-        <v>3.5960000000000001E-4</v>
+        <v>0.92300000000000004</v>
+      </c>
+      <c r="H22" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>Y</v>
+      </c>
+      <c r="I22" s="3">
+        <f t="shared" si="1"/>
+        <v>976198.93728613993</v>
       </c>
     </row>
   </sheetData>

</xml_diff>